<commit_message>
Finish tutorial steps for fake flowcell.
</commit_message>
<xml_diff>
--- a/tutorial/Barcodes_Test.xlsx
+++ b/tutorial/Barcodes_Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,25 +55,25 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">AAAAAAAAAA</t>
+    <t xml:space="preserve">AAAAAAAA</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">CCCCCCCCCC</t>
+    <t xml:space="preserve">CCCCCCCC</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">GGGGGGGGGG</t>
+    <t xml:space="preserve">GGGGGGGG</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
   </si>
   <si>
-    <t xml:space="preserve">TTTTTTTTTT</t>
+    <t xml:space="preserve">TTTTTTTT</t>
   </si>
 </sst>
 </file>
@@ -170,12 +170,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -187,13 +187,13 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,7 +274,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>